<commit_message>
[#7699] fix exited children count
</commit_message>
<xml_diff>
--- a/storage/app/excel/contact_book_1.xlsx
+++ b/storage/app/excel/contact_book_1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>001-保育園</t>
   </si>
@@ -49,7 +49,13 @@
     <t>機嫌</t>
   </si>
   <si>
+    <t>前夜</t>
+  </si>
+  <si>
     <t>午前</t>
+  </si>
+  <si>
+    <t>今朝</t>
   </si>
   <si>
     <t>午後</t>
@@ -59,6 +65,9 @@
   </si>
   <si>
     <t>睡眠</t>
+  </si>
+  <si>
+    <t>入浴</t>
   </si>
   <si>
     <t>沐浴</t>
@@ -76,9 +85,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -97,25 +106,31 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -135,13 +150,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -150,29 +158,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -203,8 +190,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -212,14 +206,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -235,6 +237,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -291,7 +300,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -303,13 +312,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -327,7 +330,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -339,7 +348,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -351,25 +360,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -381,13 +372,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -399,7 +396,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -411,49 +444,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -465,13 +480,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -599,21 +608,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -653,15 +647,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -677,11 +662,35 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -701,7 +710,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -719,130 +728,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1287,8 +1296,8 @@
   <sheetPr/>
   <dimension ref="A1:AH84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R24" sqref="R24:Y25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="O32" sqref="O32:Y33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -2090,7 +2099,7 @@
         <v>10</v>
       </c>
       <c r="O22" s="26" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="P22" s="26"/>
       <c r="Q22" s="26"/>
@@ -2152,7 +2161,7 @@
       <c r="A24" s="1"/>
       <c r="B24" s="11"/>
       <c r="C24" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
@@ -2166,7 +2175,7 @@
       <c r="M24" s="12"/>
       <c r="N24" s="11"/>
       <c r="O24" s="26" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="P24" s="26"/>
       <c r="Q24" s="26"/>
@@ -2263,7 +2272,7 @@
     <row r="27" spans="1:34">
       <c r="A27" s="1"/>
       <c r="B27" s="11" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C27" s="10" t="s">
         <v>11</v>
@@ -2279,10 +2288,10 @@
       <c r="L27" s="14"/>
       <c r="M27" s="27"/>
       <c r="N27" s="11" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="O27" s="26" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="P27" s="26"/>
       <c r="Q27" s="26"/>
@@ -2344,7 +2353,7 @@
       <c r="A29" s="1"/>
       <c r="B29" s="11"/>
       <c r="C29" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
@@ -2358,7 +2367,7 @@
       <c r="M29" s="27"/>
       <c r="N29" s="11"/>
       <c r="O29" s="26" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="P29" s="26"/>
       <c r="Q29" s="26"/>
@@ -2455,7 +2464,7 @@
     <row r="32" spans="1:34">
       <c r="A32" s="1"/>
       <c r="B32" s="11" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C32" s="14"/>
       <c r="D32" s="15"/>
@@ -2469,7 +2478,7 @@
       <c r="L32" s="15"/>
       <c r="M32" s="27"/>
       <c r="N32" s="11" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="O32" s="14"/>
       <c r="P32" s="15"/>
@@ -2639,7 +2648,7 @@
     <row r="37" spans="1:34">
       <c r="A37" s="1"/>
       <c r="B37" s="18" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C37" s="14"/>
       <c r="D37" s="15"/>
@@ -2653,7 +2662,7 @@
       <c r="L37" s="15"/>
       <c r="M37" s="27"/>
       <c r="N37" s="18" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="O37" s="14"/>
       <c r="P37" s="15"/>
@@ -2751,7 +2760,7 @@
     <row r="40" spans="1:34">
       <c r="A40" s="1"/>
       <c r="B40" s="18" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C40" s="12"/>
       <c r="D40" s="12"/>
@@ -2765,7 +2774,7 @@
       <c r="L40" s="15"/>
       <c r="M40" s="27"/>
       <c r="N40" s="18" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="O40" s="12"/>
       <c r="P40" s="12"/>
@@ -2935,7 +2944,7 @@
     <row r="45" spans="1:34">
       <c r="A45" s="1"/>
       <c r="B45" s="21" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C45" s="22"/>
       <c r="D45" s="22"/>
@@ -2949,7 +2958,7 @@
       <c r="L45" s="22"/>
       <c r="M45" s="29"/>
       <c r="N45" s="30" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="O45" s="31"/>
       <c r="P45" s="31"/>

</xml_diff>

<commit_message>
change extension type into time
</commit_message>
<xml_diff>
--- a/storage/app/excel/contact_book_1.xlsx
+++ b/storage/app/excel/contact_book_1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12495"/>
+    <workbookView windowWidth="28800" windowHeight="12495"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>001-保育園</t>
   </si>
@@ -78,16 +78,19 @@
   <si>
     <t>家庭での様子</t>
   </si>
+  <si>
+    <t>保育園での様子</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -112,16 +115,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -136,7 +139,14 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -144,7 +154,14 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -183,17 +200,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -213,7 +223,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -230,13 +240,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -300,7 +303,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -312,7 +321,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -324,13 +333,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -342,7 +411,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -354,133 +483,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -611,8 +614,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -632,6 +650,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -647,17 +674,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -679,24 +700,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -710,15 +713,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -728,130 +731,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1297,7 +1300,7 @@
   <dimension ref="A1:AH84"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="O32" sqref="O32:Y33"/>
+      <selection activeCell="N47" sqref="N47:Y53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -2958,7 +2961,7 @@
       <c r="L45" s="22"/>
       <c r="M45" s="29"/>
       <c r="N45" s="30" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O45" s="31"/>
       <c r="P45" s="31"/>

</xml_diff>